<commit_message>
implementada detecção de erros ao subir arquivos
</commit_message>
<xml_diff>
--- a/template-lista.xlsx
+++ b/template-lista.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\proti\OneDrive\Documentos\git\addon-lista-nomus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EA45F3-4346-48BF-9D68-675FFD850617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7793A3-498D-487A-A55E-2C4631C04F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2F86AC57-190D-4FCC-8330-CF613E8C50A5}"/>
+    <workbookView xWindow="3675" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{2F86AC57-190D-4FCC-8330-CF613E8C50A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,17 +54,17 @@
     <t>PROJETO</t>
   </si>
   <si>
-    <t>001.000102</t>
-  </si>
-  <si>
-    <t>001.000103</t>
+    <t>123</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +81,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,9 +144,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -178,7 +184,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -284,7 +290,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -426,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -434,68 +440,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39108D6D-CE42-4DC9-8E9D-27F6C7B9E6E4}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="21.6328125" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="30" style="3" customWidth="1"/>
-    <col min="4" max="4" width="29.08984375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.54296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="21.1796875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="19.36328125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="3"/>
+    <col min="2" max="2" width="10.6328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="3" customWidth="1"/>
+    <col min="4" max="6" width="11.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.90625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="12.26953125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.36328125" style="3" customWidth="1"/>
+    <col min="15" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>5</v>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>